<commit_message>
adds functions in NewFunctions.script and WorkbookCommandAndFunction.script
</commit_message>
<xml_diff>
--- a/Resources/Test1.xlsx
+++ b/Resources/Test1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\TSU_Excel.suite\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC0A7E2-859D-4C8A-9AAF-354E9AB41FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3EC7D6-48EE-40B2-95FB-D06297A037EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="28800" windowHeight="15460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Normalized" sheetId="1" r:id="rId1"/>
     <sheet name="Not Normalized" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="81" uniqueCount="39">
   <si>
     <t>Requirement</t>
   </si>
@@ -148,13 +148,22 @@
   </si>
   <si>
     <t>RecNumber</t>
+  </si>
+  <si>
+    <t>CourseName</t>
+  </si>
+  <si>
+    <t>CourseDate</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,21 +202,21 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="right" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -227,7 +236,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -378,7 +387,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -402,9 +411,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -428,7 +437,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -463,7 +472,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -481,7 +490,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -506,7 +515,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -542,23 +551,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08CC13A-FEA9-4C08-B151-AFB39DB95A3A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08CC13A-FEA9-4C08-B151-AFB39DB95A3A}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" s="1" customFormat="true" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +587,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -595,7 +604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -612,7 +621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -629,7 +638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -646,7 +655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -663,7 +672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -680,7 +689,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -697,7 +706,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -720,23 +729,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6346BD20-AEED-4134-A4D0-B0BB5C1B2F00}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6346BD20-AEED-4134-A4D0-B0BB5C1B2F00}">
   <dimension ref="A3:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="53.54296875" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="14" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="11.26953125" style="4" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="11" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" s="1" customFormat="true" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -744,22 +753,22 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -778,8 +787,11 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -798,8 +810,11 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -818,8 +833,11 @@
       <c r="F6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -838,8 +856,11 @@
       <c r="F7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -858,8 +879,11 @@
       <c r="F8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" ht="29" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -878,8 +902,11 @@
       <c r="F9" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7</v>
       </c>
@@ -898,8 +925,11 @@
       <c r="F10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>8</v>
       </c>
@@ -917,6 +947,9 @@
       </c>
       <c r="F11" t="s">
         <v>8</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>